<commit_message>
[Feature] Add all indicators (points and forms indicators) by report
</commit_message>
<xml_diff>
--- a/public/importExcel/marcoJuridico/notAdminDependenciasJuridico.xlsx
+++ b/public/importExcel/marcoJuridico/notAdminDependenciasJuridico.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>id_dependencia</t>
   </si>
@@ -39,7 +39,7 @@
     <t>Contraloria</t>
   </si>
   <si>
-    <t xml:space="preserve">Por este medio reciba un cordial saludo y, al mismo tiempo, con fundamento en lo dispuesto en los artículos 115 de la Constitución Política de los Estados Unidos Mexicanos; 102, 103 y 105 de la Constitución Política del Estado Libre y Soberano de Puebla; 2, 3, 4, 78, 118, 119, 120, 122, 123, 168 y 169 de la Ley Orgánica Municipal; 11 y 13 fracción XI del Reglamento Interior de la Contraloría Municipal del Honorable Ayuntamiento del Municipio de Puebla y, en seguimiento a la &lt;strong&gt;CIRCULAR [numDocument]&lt;/strong&gt;, de fecha [completeDate], recibida en la Oficialía de Partes de este Órgano Interno de Control el día 3 de igual mes y año, en la cual señala las fechas, lineamientos y criterios que se deberán seguir para la remisión de la &lt;strong&gt;NOTICIA ADMINISTRATIVA&lt;/strong&gt; correspondiente al año [year]; dicho lo anterior, anexo al presente la información debidamente requisitada al corte del mes de [monthYear].
+    <t xml:space="preserve">&amp;nbsp;Por este medio reciba un cordial saludo y, al mismo tiempo, con fundamento en lo dispuesto en los artículos 115 de la Constitución Política de los Estados Unidos Mexicanos; 102, 103 y 105 de la Constitución Política del Estado Libre y Soberano de Puebla; 2, 3, 4, 78, 118, 119, 120, 122, 123, 168 y 169 de la Ley Orgánica Municipal; 11 y 13 fracción XI del Reglamento Interior de la Contraloría Municipal del Honorable Ayuntamiento del Municipio de Puebla y, en seguimiento a la &lt;strong&gt;CIRCULAR [numDocument]&lt;/strong&gt;, de fecha [completeDate], recibida en la Oficialía de Partes de este Órgano Interno de Control el día 3 de igual mes y año, en la cual señala las fechas, lineamientos y criterios que se deberán seguir para la remisión de la &lt;strong&gt;NOTICIA ADMINISTRATIVA&lt;/strong&gt; correspondiente al año [year]; dicho lo anterior, anexo al presente la información debidamente requisitada al corte del mes de [monthYear].
 </t>
   </si>
   <si>
@@ -52,7 +52,7 @@
   </si>
   <si>
     <t>Con fundamento en el artículo 9 del Reglamento Interior de la Coordinación de las Regidurías del Honorable Ayuntamiento del Municipio de Puebla, en respuesta al OFICIO [numDocument], remito a usted la Noticia Administrativa y Estadística de la Coordinación de las Regidurías, correspondiente al mes de [monthYear].
-No omito mencionar que dicha información se anexa al presente de forma impresa y editable por correo electrónico.</t>
+&amp;nbsp;No omito mencionar que dicha información se anexa al presente de forma impresa y editable por correo electrónico.</t>
   </si>
   <si>
     <t>“Mira de cerca al presente que estás construyendo, porque debe parecerse al futuro con el que sueñas” Norma Palafox
@@ -102,7 +102,7 @@
   </si>
   <si>
     <t>Por medio del presente reciba un cordial saludo, al mismo tiempo en términos de lo dispuesto en los artículos 91 fracción XXXVII y 138 de la Ley Orgánica Municipal; Artículos 6, 8 y 11 fracción II y XV del Reglamento Interior de la Secretaría para la Igualdad Sustantiva de Género, me permito remitir la Noticia Administrativa correspondiente al mes de [month] de la dependencia a mi cargo, para los efectos conducentes.
-Así mismo, no omito mencionar que en este mes no se agregaron conceptos nuevos en ninguna de las 2 unidades administrativas.</t>
+&amp;nbsp;Así mismo, no omito mencionar que en este mes no se agregaron conceptos nuevos en ninguna de las 2 unidades administrativas.</t>
   </si>
   <si>
     <t xml:space="preserve">“Mira de cerca al presente que estas construyendo, porque debe parecerse al futuro con el que sueñas” (Norma Palafox)
@@ -168,11 +168,11 @@
   </si>
   <si>
     <t>Con fundamento en el artículo 13, fracciones XIV y XV, del Reglamento Interior de la Secretaría de Economía y Turismo del Honorable Ayuntamiento del Municipio de Puebla, por instrucciones del Secretario de Economía y Turismo, me permito anexar al presente la Noticia Administrativa correspondiente al mes de [monthYear], en la que se incluyen los nuevos conceptos que se desglosan a continuación:
-    • Dirección de Turismo
-1.- LA 57 Realizar 2 participaciones en asambleas de trabajo de Redes Gastronómicas.
-2.- LA 49 Obtener 2 constancias de capacitación para personal relacionado al turismo (servidores públicos, miembros del sector turístico, entre otros).
-    • Coordinación de Promoción
-4.- LA 3 Gestionar 1 sistema de análisis de información para la promoción y atracción de inversiones (Emblemática).</t>
+&amp;nbsp;• Dirección de Turismo
+&amp;nbsp;&amp;nbsp;&amp;nbsp;1.- LA 57 Realizar 2 participaciones en asambleas de trabajo de Redes Gastronómicas.
+&amp;nbsp;&amp;nbsp;&amp;nbsp;2.- LA 49 Obtener 2 constancias de capacitación para personal relacionado al turismo (servidores públicos, miembros del sector turístico, entre otros).
+&amp;nbsp;• Coordinación de Promoción
+&amp;nbsp;&amp;nbsp;&amp;nbsp;4.- LA 3 Gestionar 1 sistema de análisis de información para la promoción y atracción de inversiones (Emblemática).</t>
   </si>
   <si>
     <t>“La experiencia te hace entender que jugando en equipo y siendo solidario se alcanzan mayores objetivos” (Cristiano Ronaldo). 
@@ -182,7 +182,7 @@
     <t>Secretaría de Seguridad Ciudadana</t>
   </si>
   <si>
-    <t>Con fundamento en los artículos 21 párrafo octavo de la Constitución Política de los Estados Unidos Mexicanos; 16 y 18 fracciones XI y XXXIX del Reglamento Interior de la Secretaría de Seguridad Ciudadana del Honorable Ayuntamiento del Municipio de Puebla, y con base en el MEMORANDÚM [numDocument], asignado por el Coronel Retirado Braulio Fernando Domínguez Torres, Director de Planeación y Aseguramiento de Objetivos y Metas de esta Secretaría a mi cargo, en el que remite lo respectivo a la Noticia Administrativa; me permito informar a Usted (anexo al presente) dichos resultados obtenidos durante el mes de [month] del año en curso, por las diversas áreas de esta Secretaría.</t>
+    <t>&amp;nbsp;Con fundamento en los artículos 21 párrafo octavo de la Constitución Política de los Estados Unidos Mexicanos; 16 y 18 fracciones XI y XXXIX del Reglamento Interior de la Secretaría de Seguridad Ciudadana del Honorable Ayuntamiento del Municipio de Puebla, y con base en el MEMORANDÚM [numDocument], asignado por el Coronel Retirado Braulio Fernando Domínguez Torres, Director de Planeación y Aseguramiento de Objetivos y Metas de esta Secretaría a mi cargo, en el que remite lo respectivo a la Noticia Administrativa; me permito informar a Usted (anexo al presente) dichos resultados obtenidos durante el mes de [month] del año en curso, por las diversas áreas de esta Secretaría.</t>
   </si>
   <si>
     <t>“Mira de cerca al presente que estás construyendo, porque debe parecerse al futuro con el que sueñas”. Norma Palafox. “Se testigo de un gran evento, Torneo Mundial de Fútbol 7 en Puebla.”</t>
@@ -192,7 +192,7 @@
   </si>
   <si>
     <t xml:space="preserve">Con fundamento en lo establecido por los Artículos 118, 120, 122 y 123 de la Ley Orgánica Municipal; 6, 10 fracción XLVII, 12 fracción XVII y 13 fracción XXII del Reglamento Interior de la Secretaría de Movilidad e Infraestructura del Honorable Ayuntamiento del Municipio de Puebla, y en cumplimiento a la &lt;strong&gt;CIRCULAR [numDocument]&lt;/strong&gt; de [semiDate] del año en curso, respetuosamente se informa que, de manera adjunta al presente, &lt;strong&gt;se remite la información de la Noticia Administrativa y Estadística correspondiente al mes de [monthYear], de las áreas que conforman la Secretaría de Movilidad e Infraestructura&lt;/strong&gt; del H. Ayuntamiento del Municipio de Puebla.
-Cabe precisar que en la Noticia Administrativa y Estadística de este mes &lt;strong&gt;no se incluye algún nuevo concepto.&lt;/strong&gt; </t>
+&amp;nbsp;Cabe precisar que en la Noticia Administrativa y Estadística de este mes &lt;strong&gt;no se incluye algún nuevo concepto.&lt;/strong&gt; </t>
   </si>
   <si>
     <t>“Mira de cerca al presente que estás construyendo, porque debe parecerse al futuro con el que sueñas”
@@ -214,7 +214,7 @@
   </si>
   <si>
     <t>Reciba un cordial saludo y con fundamento en lo dispuesto en el artículo 115 de la Constitución Política de los Estados Unidos Mexicanos, 102 de la Constitución Política para el Estado Libre y Soberano de Puebla; 100 fracciones I y XVIII de la Ley Orgánica Municipal; 8 fracción I y X, y 11 fracciones III, XX, XIV, y LXI del Reglamento Interior de la Sindicatura Municipal del Honorable Ayuntamiento del Municipio de Puebla, en seguimiento a su Circular [numDocument] de fecha [semiDate] del presente año, al cual se le asignó el número de folio interno 000065, de la manera más atenta, me permito remitir a usted:
-Noticia Administrativa correspondiente al mes de [monthYear].</t>
+&amp;nbsp;Noticia Administrativa correspondiente al mes de [monthYear].</t>
   </si>
   <si>
     <t>"Mira de cerca al presente que estas construyendo, porque debe parecerse al futuro con el que sueñas”. Norma Palafox. “Se testigo de un gran evento, Torneo Mundial de Fútbol 7 en Puebla”.</t>
@@ -241,6 +241,19 @@
   <si>
     <t>“Mira de cerca al presente que estas construyendo, porque debe parecerse al futuro con el que sueñas”                    
   (Norma Palafox)” Sé testigo de un gran evento, Torneo Mundial de Fútbol 7 en Puebla”</t>
+  </si>
+  <si>
+    <t>Secretaría de Bienestar y Participación Ciudadana</t>
+  </si>
+  <si>
+    <t>Con fundamento en lo dispuesto en los artículos 118,119 y 120 de la Ley Orgánica Municipal; 9, 10 y 11 fracciones I, II y XLIII del Reglamento Interior de la Secretaria de Bienestar y Participación Ciudadana del Honorable Ayuntamiento del Municipio de Puebla; adjunto para los efectos conducentes, la Noticia Administrativa correspondiente al mes de junio del ejercicio [year], relativa a esta Secretaria.</t>
+  </si>
+  <si>
+    <t>Secretaría de Medio Ambiente</t>
+  </si>
+  <si>
+    <t>Con fundamento en lo establecido por el artículo 11 fracciones VII, XVI y XVIII del Reglamento Interior de la Secretaría de Medio Ambiente del Honorable Ayuntamiento del Municipio de Puebla y, en atención a la circular identificada con el [numDocument], mediante la cual se informa sobre el calendario con las fechas correspondientes a la entrega de la Noticia Administrativa del año [year], a la Dependencia a su digno cargo, se hace de su conocimiento lo siguiente:
+&amp;nbsp;Se anexa al presente el informe correspondiente a la Noticia Administrativa de esta Secretaría, correspondiente al mes de [monthYear].</t>
   </si>
   <si>
     <t>[numDocument] =  NÚM. SA-030/2023
@@ -805,7 +818,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>58</v>
@@ -832,10 +845,32 @@
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="4"/>
+      <c r="A23" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24">
-      <c r="C24" s="4"/>
+      <c r="A24" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25">
       <c r="C25" s="4"/>
@@ -843,7 +878,7 @@
     <row r="26">
       <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27">

</xml_diff>